<commit_message>
created excel management system
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -391,7 +391,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:F2"/>
@@ -402,33 +402,48 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>No.</t>
+          <t>Mail</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Mail</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Pass</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
           <t>Saldo</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>bagas@mail.com</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Bagas</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
@@ -442,71 +457,251 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="19" customWidth="1" min="1" max="1"/>
+    <col width="20.7109375" customWidth="1" min="2" max="2"/>
+    <col width="20.28515625" customWidth="1" min="4" max="4"/>
+    <col width="18.140625" customWidth="1" min="5" max="5"/>
+    <col width="14.42578125" customWidth="1" min="8" max="8"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>No.</t>
+          <t>Time In</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Time In</t>
+          <t>Gate In</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Gate In</t>
+          <t>KM In</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>KM In</t>
+          <t>Time Out</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Time Out</t>
+          <t>Gate Out</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Gate Out</t>
+          <t>KM Out</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>KM Out</t>
+          <t>Jarak</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Jarak</t>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Golongan</t>
         </is>
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>11:35:33</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>semarang</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>12</v>
-      </c>
-      <c r="G2" t="n">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <f>ABS($G$2 - $D$2)</f>
-        <v/>
+          <t>Semarang</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>11:35:33</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Serpong</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>11:38:45</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Juanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>11:38:45</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Solo</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>bagas@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>12:09:47</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Semarang</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>12:09:47</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Taman Mini</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>test2@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>12:18:25</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Tambak Sumur</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>12:18:25</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Tanjung Priok</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>12:23:34</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Tambak Oso</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>12:23:34</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Juanda</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>test1@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>12:37:13</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Bawen</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>23.1</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>12:37:13</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Taman Mini</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H8" t="n">
+        <v>473.6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>12:44:40</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Bawen</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>12:44:40</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Taman Mini</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>test2@mail.com</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated layout and km masuk keluar
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -3,10 +3,10 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="user" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="database user" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="log" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
@@ -402,10 +402,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -461,9 +461,28 @@
         <v>10000</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>test1@mail.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E3" t="n">
+        <v>12000</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -475,10 +494,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H7:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -682,21 +701,271 @@
     <row r="7">
       <c r="H7" t="inlineStr">
         <is>
-          <t>test1@mail.com</t>
+          <t>bagas@mail.com</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="H8" t="inlineStr">
         <is>
-          <t>bagas@mail.com</t>
+          <t>test1@mail.com</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="H9" t="inlineStr">
         <is>
+          <t>test1@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>test1@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>test1@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>21:59:21</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Bawen</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>21:59:21</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Taman Mini</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>test1@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>22:02:11</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Tambak Sumur</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>22:02:12</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Juanda</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
           <t>bagas@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>22:11:07</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Solo</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>bagas@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>22:23:35</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Semarang</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>22:23:35</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Tanjung Priok</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>5</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>bagas@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>22:28:37</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Tanjung Priok</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>5</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>22:28:37</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Juanda</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>bagas@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>22:30:36</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Tambak Oso</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>22:30:36</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Solo</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>40</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>bagas@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>22:34:40</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Tambak Sumur</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>5</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>22:34:40</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Taman Mini</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>test1@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>22:39:22</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Tambak Oso</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>22:39:22</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Juanda</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>9</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>test1@mail.com</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
coba update hasil page
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -408,7 +408,7 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="20.7109375" customWidth="1" min="1" max="1"/>
     <col width="19.42578125" customWidth="1" min="2" max="2"/>
@@ -458,7 +458,7 @@
         <v>123456</v>
       </c>
       <c r="E2" t="n">
-        <v>10000</v>
+        <v>22000</v>
       </c>
     </row>
     <row r="3">
@@ -494,13 +494,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A8" sqref="A8:L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="19" customWidth="1" min="1" max="1"/>
     <col width="20.7109375" customWidth="1" min="2" max="2"/>
@@ -762,41 +762,83 @@
       </c>
     </row>
     <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>13:31:23</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Solo</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>40</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>13:31:23</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Serpong</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>10.1</v>
+      </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>test1@mail.com</t>
+          <t>bagas@mail.com</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Semarang</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Jakarta</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>19030</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>01:17:23</t>
+          <t>13:34:36</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Serpong</t>
+          <t>Bawen</t>
         </is>
       </c>
       <c r="C9" t="n">
+        <v>23.1</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>13:34:36</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Tanjung Priok</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
         <v>12.1</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>01:17:23</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Taman Mini</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>4.5</v>
+      <c r="G9" t="n">
+        <v>481.2</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -804,511 +846,20 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
+          <t>Semarang</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
           <t>Jakarta</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Jakarta</t>
-        </is>
-      </c>
       <c r="L9" t="n">
-        <v>4980</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>01:35:35</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Serpong</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>12.1</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>01:35:35</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Solo</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>40</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>bagas@mail.com</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Jakarta</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>Semarang</t>
-        </is>
-      </c>
-      <c r="L10" t="n">
-        <v>19630</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>01:38:25</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Bawen</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>23.1</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>01:38:25</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Taman Mini</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>test1@mail.com</t>
-        </is>
-      </c>
-      <c r="I11" t="n">
-        <v>2</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Semarang</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Jakarta</t>
-        </is>
-      </c>
-      <c r="L11" t="n">
-        <v>10590</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>01:42:08</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Tanjung Priok</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>10.1</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>01:42:09</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Juanda</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>9</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>test1@mail.com</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Jakarta</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>Surabaya</t>
-        </is>
-      </c>
-      <c r="L12" t="n">
-        <v>7080</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>01:46:44</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Serpong</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>12.1</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>01:46:44</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Juanda</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>9</v>
-      </c>
-      <c r="G13" t="n">
-        <v>818.1</v>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>bagas@mail.com</t>
-        </is>
-      </c>
-      <c r="I13" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Jakarta</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>Surabaya</t>
-        </is>
-      </c>
-      <c r="L13" t="n">
-        <v>7680</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>07:13:53</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Tambak Sumur</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>5</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>07:13:53</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Juanda</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
-        <v>9</v>
-      </c>
-      <c r="G14" t="n">
-        <v>14</v>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>test1@mail.com</t>
-        </is>
-      </c>
-      <c r="I14" t="n">
-        <v>1</v>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Surabaya</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>Surabaya</t>
-        </is>
-      </c>
-      <c r="L14" t="n">
-        <v>6300</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>08:48:47</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Tambak Sumur</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>5</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>08:48:47</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Taman Mini</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="G15" t="n">
-        <v>806.5</v>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>test1@mail.com</t>
-        </is>
-      </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>Surabaya</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>Jakarta</t>
-        </is>
-      </c>
-      <c r="L15" t="n">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>08:51:33</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Tambak Sumur</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>5</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>08:51:33</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Taman Mini</t>
-        </is>
-      </c>
-      <c r="F16" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>bagas@mail.com</t>
-        </is>
-      </c>
-      <c r="I16" t="n">
-        <v>1</v>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>Surabaya</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>Jakarta</t>
-        </is>
-      </c>
-      <c r="L16" t="n">
-        <v>4950</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>09:31:20</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Tambak Sumur</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>5</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>09:31:20</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Taman Mini</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="G17" t="n">
-        <v>806.5</v>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>test1@mail.com</t>
-        </is>
-      </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>Surabaya</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>Jakarta</t>
-        </is>
-      </c>
-      <c r="L17" t="n">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>09:33:34</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Juanda</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>12.8</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>09:33:34</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Tanjung Priok</t>
-        </is>
-      </c>
-      <c r="F18" t="n">
-        <v>12.1</v>
-      </c>
-      <c r="G18" t="n">
-        <v>821.9</v>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>test1@mail.com</t>
-        </is>
-      </c>
-      <c r="I18" t="n">
-        <v>1</v>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>Surabaya</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>Jakarta</t>
-        </is>
-      </c>
-      <c r="L18" t="n">
-        <v>699640</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>bagas@mail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>bagas@mail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>test1@mail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>test1@mail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>bagas@mail.com</t>
-        </is>
+        <v>548070</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created page 6 and quit button
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -458,7 +458,7 @@
         <v>123456</v>
       </c>
       <c r="E2" t="n">
-        <v>67550</v>
+        <v>14610</v>
       </c>
     </row>
     <row r="3">
@@ -476,7 +476,7 @@
         <v>123456</v>
       </c>
       <c r="E3" t="n">
-        <v>58000</v>
+        <v>48760</v>
       </c>
     </row>
     <row r="4">
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>624170</v>
+        <v>199290</v>
       </c>
     </row>
   </sheetData>
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:L26"/>
@@ -1727,6 +1727,318 @@
         <v>1051260</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>20:38:24</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Taman Mini</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>20:38:24</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Tambak Sumur</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>5</v>
+      </c>
+      <c r="G33" t="n">
+        <v>806.5</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>bagas@mail.com</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Jakarta</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Surabaya</t>
+        </is>
+      </c>
+      <c r="L33" t="n">
+        <v>693850</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>20:41:52</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Semarang</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>20:41:52</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Taman Mini</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="G34" t="n">
+        <v>450.5</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>bagas@mail.com</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>1</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Semarang</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Jakarta</t>
+        </is>
+      </c>
+      <c r="L34" t="n">
+        <v>358150</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>20:47:04</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Juanda</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>20:47:04</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Serpong</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>10.1</v>
+      </c>
+      <c r="G35" t="n">
+        <v>819.9</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>bagas@mail.com</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>2</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Surabaya</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Jakarta</t>
+        </is>
+      </c>
+      <c r="L35" t="n">
+        <v>1052940</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>20:55:04</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Semarang</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>20:55:04</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Bawen</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>23.1</v>
+      </c>
+      <c r="G36" t="n">
+        <v>23.1</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>test1@mail.com</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>2</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Semarang</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Semarang</t>
+        </is>
+      </c>
+      <c r="L36" t="n">
+        <v>9240</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>21:06:11</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Juanda</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>21:06:11</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Tanjung Priok</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="G37" t="n">
+        <v>821.9</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>zaki@mail.com</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>1</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Surabaya</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Jakarta</t>
+        </is>
+      </c>
+      <c r="L37" t="n">
+        <v>699640</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>21:09:58</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Bawen</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>23.1</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>21:09:58</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Solo</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>40</v>
+      </c>
+      <c r="G38" t="n">
+        <v>63.1</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>zaki@mail.com</t>
+        </is>
+      </c>
+      <c r="I38" t="n">
+        <v>2</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Semarang</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Semarang</t>
+        </is>
+      </c>
+      <c r="L38" t="n">
+        <v>25240</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>